<commit_message>
Added more level generator stuff
</commit_message>
<xml_diff>
--- a/Levels/level_generators/level1/o_level1.xlsx
+++ b/Levels/level_generators/level1/o_level1.xlsx
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:Q19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1077,10 +1077,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
@@ -1116,10 +1116,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>2</v>
@@ -1155,13 +1155,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Edited levels to add locked and unlocked doors, as well as key walls. Changed README.md to modify the additions, and removed the level template for now
</commit_message>
<xml_diff>
--- a/Levels/level_generators/level1/o_level1.xlsx
+++ b/Levels/level_generators/level1/o_level1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10240" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="8880" yWindow="460" windowWidth="10240" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="o_level1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="9">
   <si>
     <t>P</t>
   </si>
@@ -41,9 +41,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>S(D)</t>
+  </si>
+  <si>
+    <t>D(L)</t>
+  </si>
+  <si>
+    <t>KW</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,103 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -719,7 +818,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -882,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>2</v>
@@ -996,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>1</v>
@@ -1080,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
@@ -1113,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
@@ -1155,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
@@ -1173,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>2</v>
@@ -1306,47 +1405,55 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:P16">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="S(D)">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="S(D)">
       <formula>NOT(ISERROR(SEARCH("S(D)",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="L">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="L">
       <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="L">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="L">
       <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="#">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="#">
       <formula>NOT(ISERROR(SEARCH("#",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="K">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="K">
       <formula>NOT(ISERROR(SEARCH("K",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="_">
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="_">
       <formula>NOT(ISERROR(SEARCH("_",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="14" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="D(L)">
+      <formula>NOT(ISERROR(SEARCH("D(L)",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="KW">
+      <formula>NOT(ISERROR(SEARCH("KW",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edited level fetcher to convert the borad to instances of objects before returning it. Deleted unnecessary pycache files and random extra excel temp iles. Changes Game-elements to add state changing to switches and added doors. (aka: yo)
</commit_message>
<xml_diff>
--- a/Levels/level_generators/level1/o_level1.xlsx
+++ b/Levels/level_generators/level1/o_level1.xlsx
@@ -104,31 +104,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color theme="1"/>
@@ -136,30 +112,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
       <border>
@@ -818,7 +770,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1209,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -1405,54 +1357,54 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:P16">
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="S(D)">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="S(D)">
       <formula>NOT(ISERROR(SEARCH("S(D)",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="L">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="L">
       <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="L">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="L">
       <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="#">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="#">
       <formula>NOT(ISERROR(SEARCH("#",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="K">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="K">
       <formula>NOT(ISERROR(SEARCH("K",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="_">
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="_">
       <formula>NOT(ISERROR(SEARCH("_",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="D(L)">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="D(L)">
       <formula>NOT(ISERROR(SEARCH("D(L)",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="KW">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="KW">
       <formula>NOT(ISERROR(SEARCH("KW",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Modified drawing code so that we only draw things that moved, and remove sprites of things when we move away (which speeds stuff up a ton). Also changed collision code. I think it looks a little cleaner now. And made a function so that game elements can update their own states based on the world around them (keywalls stop being solid, doors unlock, etc)
</commit_message>
<xml_diff>
--- a/Levels/level_generators/level1/o_level1.xlsx
+++ b/Levels/level_generators/level1/o_level1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="460" windowWidth="10240" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="660" windowWidth="20080" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="o_level1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="9">
-  <si>
-    <t>P</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="3">
   <si>
     <t>W</t>
   </si>
@@ -39,21 +36,6 @@
   </si>
   <si>
     <t>K</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>S(D)</t>
-  </si>
-  <si>
-    <t>D(L)</t>
-  </si>
-  <si>
-    <t>KW</t>
   </si>
 </sst>
 </file>
@@ -770,7 +752,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,40 +762,40 @@
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -822,40 +804,40 @@
     </row>
     <row r="2" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -864,40 +846,40 @@
     </row>
     <row r="3" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -906,40 +888,40 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -948,40 +930,40 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -990,40 +972,40 @@
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1032,40 +1014,40 @@
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1074,40 +1056,40 @@
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1116,40 +1098,40 @@
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1158,40 +1140,40 @@
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1200,40 +1182,40 @@
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1242,40 +1224,40 @@
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>

</xml_diff>